<commit_message>
Arrumando comentario, tests , nome de metodos
</commit_message>
<xml_diff>
--- a/Docs/PlanilhasDeTeste/ContratoMustPassVerificandoAdicionandoPlanoContratadoEmContratoExistene.xlsx
+++ b/Docs/PlanilhasDeTeste/ContratoMustPassVerificandoAdicionandoPlanoContratadoEmContratoExistene.xlsx
@@ -47,7 +47,7 @@
     <t xml:space="preserve">Dias da semana *</t>
   </si>
   <si>
-    <t xml:space="preserve">Henrique nitatori</t>
+    <t xml:space="preserve">Henrique dos santos</t>
   </si>
   <si>
     <t xml:space="preserve">Plano - Psicologia</t>
@@ -319,7 +319,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="bottomRight" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>